<commit_message>
Finish part of sheriff evaluaiton
</commit_message>
<xml_diff>
--- a/sheriff/figure/sheriffoverhead.xlsx
+++ b/sheriff/figure/sheriffoverhead.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="12740" windowHeight="12700" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="20760" windowHeight="13460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="perf" sheetId="7" r:id="rId1"/>
+    <sheet name="perf " sheetId="11" r:id="rId1"/>
+    <sheet name="sensitivity" sheetId="9" r:id="rId2"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -19,45 +20,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="25">
-  <si>
-    <t>canneal</t>
-  </si>
-  <si>
-    <t>dedup</t>
-  </si>
-  <si>
-    <t>streamcluster</t>
-  </si>
-  <si>
-    <t>blackscholes</t>
-  </si>
-  <si>
-    <t>swaptions</t>
-  </si>
-  <si>
-    <t>histogram</t>
-  </si>
-  <si>
-    <t>kmeans</t>
-  </si>
-  <si>
-    <t>linear_regression</t>
-  </si>
-  <si>
-    <t>matrix_multiply</t>
-  </si>
-  <si>
-    <t>pca</t>
-  </si>
-  <si>
-    <t>reverse_index</t>
-  </si>
-  <si>
-    <t>string_match</t>
-  </si>
-  <si>
-    <t>word_count</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="47">
+  <si>
+    <t>2ms</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>geomean</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>pfscan</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>pbzip2</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>fluidanimate</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ferret</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>pthreads</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>pfscan</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>pbzip2</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>fluidanimate</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ferret</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>pthreads</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
     <t>DETECTIVE</t>
@@ -68,7 +78,46 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>pthreads</t>
+    <t>canneal</t>
+  </si>
+  <si>
+    <t>dedup</t>
+  </si>
+  <si>
+    <t>streamcluster</t>
+  </si>
+  <si>
+    <t>blackscholes</t>
+  </si>
+  <si>
+    <t>swaptions</t>
+  </si>
+  <si>
+    <t>histogram</t>
+  </si>
+  <si>
+    <t>kmeans</t>
+  </si>
+  <si>
+    <t>linear_regression</t>
+  </si>
+  <si>
+    <t>matrix_multiply</t>
+  </si>
+  <si>
+    <t>pca</t>
+  </si>
+  <si>
+    <t>reverse_index</t>
+  </si>
+  <si>
+    <t>string_match</t>
+  </si>
+  <si>
+    <t>word_count</t>
+  </si>
+  <si>
+    <t>DETECTIVE</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -84,27 +133,123 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>pbzip2</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>pfscan</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>FS-PATROL</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>FS-DETECTIVE</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>X</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>X</t>
+    <t>10ms</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>10ms</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>50ms</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2ms</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>50ms</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>50ms-objects</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>(one object is changed)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>50ms-writes</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>10ms-writes</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>10ms-objects</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2ms-writes</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2ms-objects</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>HERIFF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-P</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>ROTECT</t>
+    </r>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>S</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>HERIFF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>ETECT</t>
+    </r>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -112,13 +257,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -165,6 +304,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -188,9 +332,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -206,6 +349,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -238,15 +385,31 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1400"/>
-              <a:t>FS-</a:t>
+              <a:t>S</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>HERIFF</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>-</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1400" cap="small"/>
-              <a:t>Patrol</a:t>
+              <a:t>P</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" cap="small"/>
+              <a:t>ROTECT</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" cap="all"/>
+              <a:t> </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1400" baseline="0"/>
-              <a:t> performance</a:t>
+              <a:t>performance</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1400"/>
           </a:p>
@@ -267,10 +430,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1085026849559"/>
-          <c:y val="0.143960972269771"/>
-          <c:w val="0.868529117164241"/>
-          <c:h val="0.486597436190041"/>
+          <c:x val="0.0694440846528026"/>
+          <c:y val="0.119504463315695"/>
+          <c:w val="0.919605671514923"/>
+          <c:h val="0.535510584507723"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -281,7 +444,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>perf!$G$1</c:f>
+              <c:f>'perf '!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -302,7 +465,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>perf!$F$2:$F$20</c:f>
+              <c:f>'perf '!$F$2:$F$20</c:f>
               <c:strCache>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
@@ -364,7 +527,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>perf!$G$2:$G$20</c:f>
+              <c:f>'perf '!$G$2:$G$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -431,11 +594,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>perf!$H$1</c:f>
+              <c:f>'perf '!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>FS-PATROL</c:v>
+                  <c:v>SHERIFF-PROTECT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -450,7 +613,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>perf!$F$2:$F$20</c:f>
+              <c:f>'perf '!$F$2:$F$20</c:f>
               <c:strCache>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
@@ -512,7 +675,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>perf!$H$2:$H$20</c:f>
+              <c:f>'perf '!$H$2:$H$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="19"/>
@@ -574,11 +737,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="523898648"/>
-        <c:axId val="523958728"/>
+        <c:axId val="583182888"/>
+        <c:axId val="583186216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="523898648"/>
+        <c:axId val="583182888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -594,7 +757,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="523958728"/>
+        <c:crossAx val="583186216"/>
         <c:crossesAt val="0.0"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -602,7 +765,7 @@
         <c:tickMarkSkip val="9"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="523958728"/>
+        <c:axId val="583186216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.75"/>
@@ -635,7 +798,7 @@
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="523898648"/>
+        <c:crossAx val="583182888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.25"/>
@@ -693,11 +856,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1400" baseline="0"/>
-              <a:t>FS-</a:t>
+              <a:t>S</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="1400" cap="small" baseline="0"/>
-              <a:t>Detective</a:t>
+              <a:rPr lang="en-US" sz="1200" cap="small" baseline="0"/>
+              <a:t>HERIFF</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t>-D</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" baseline="0"/>
+              <a:t>ETECT</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1400" baseline="0"/>
@@ -722,10 +893,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1085026849559"/>
-          <c:y val="0.143960972269771"/>
-          <c:w val="0.868529117164241"/>
-          <c:h val="0.486597436190041"/>
+          <c:x val="0.0640582825833024"/>
+          <c:y val="0.136288406613572"/>
+          <c:w val="0.922695765234496"/>
+          <c:h val="0.524960692833182"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -736,7 +907,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>perf!$B$22</c:f>
+              <c:f>'perf '!$B$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -757,7 +928,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>perf!$A$23:$A$41</c:f>
+              <c:f>'perf '!$A$23:$A$41</c:f>
               <c:strCache>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
@@ -819,7 +990,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>perf!$B$23:$B$41</c:f>
+              <c:f>'perf '!$B$23:$B$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
@@ -886,11 +1057,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>perf!$C$22</c:f>
+              <c:f>'perf '!$C$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>FS-DETECTIVE</c:v>
+                  <c:v>SHERIFF-DETECT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -923,7 +1094,7 @@
           </c:dPt>
           <c:cat>
             <c:strRef>
-              <c:f>perf!$A$23:$A$41</c:f>
+              <c:f>'perf '!$A$23:$A$41</c:f>
               <c:strCache>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
@@ -985,7 +1156,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>perf!$C$23:$C$41</c:f>
+              <c:f>'perf '!$C$23:$C$41</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="19"/>
@@ -1047,11 +1218,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="481215000"/>
-        <c:axId val="480350056"/>
+        <c:axId val="583260952"/>
+        <c:axId val="583264280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="481215000"/>
+        <c:axId val="583260952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1067,7 +1238,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="480350056"/>
+        <c:crossAx val="583264280"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1075,7 +1246,7 @@
         <c:tickMarkSkip val="9"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="480350056"/>
+        <c:axId val="583264280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.0"/>
@@ -1107,7 +1278,7 @@
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="481215000"/>
+        <c:crossAx val="583260952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.5"/>
@@ -1121,8 +1292,605 @@
           <c:yMode val="edge"/>
           <c:x val="0.410208507195045"/>
           <c:y val="0.910857538140412"/>
-          <c:w val="0.16672277438577"/>
+          <c:w val="0.190333859324818"/>
           <c:h val="0.0495422284543199"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Sensitivity</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t> To </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Sampling</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t> Rate</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.373380878659583"/>
+          <c:y val="0.00280447560671097"/>
+        </c:manualLayout>
+      </c:layout>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0694440764384251"/>
+          <c:y val="0.107276166707428"/>
+          <c:w val="0.921107934167719"/>
+          <c:h val="0.543662584803452"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>sensitivity!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2ms</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="12700">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>sensitivity!$H$2:$H$19</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>blackscholes</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>dedup</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ferret</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>fluidanimate</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>histogram</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>linear_regression</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>matrix_multiply</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>pca</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>pfscan</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>streamcluster</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>string_match</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>swaptions</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>word_count</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>geomean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>sensitivity!$I$2:$I$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1.001568532818533</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.263145756457564</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.00287356328161</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.969812925170068</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.95565749235474</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.001823819077148</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.003289473928947</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.057505257623554</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.01626111370613</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.983561643835616</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.9804913295</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.976384364840391</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.001201923086538</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.004889975547677</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.0046875</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.00312680420579</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>sensitivity!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10ms</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>sensitivity!$H$2:$H$19</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>blackscholes</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>dedup</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ferret</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>fluidanimate</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>histogram</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>linear_regression</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>matrix_multiply</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>pca</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>pfscan</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>streamcluster</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>string_match</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>swaptions</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>word_count</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>geomean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>sensitivity!$J$2:$J$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>sensitivity!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>50ms</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="85000"/>
+                <a:lumOff val="15000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:strRef>
+              <c:f>sensitivity!$H$2:$H$19</c:f>
+              <c:strCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>blackscholes</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>canneal</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>dedup</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>ferret</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>fluidanimate</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>histogram</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>kmeans</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>linear_regression</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>matrix_multiply</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>pca</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>pfscan</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>reverse_index</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>streamcluster</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>string_match</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>swaptions</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>word_count</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>geomean</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>sensitivity!$K$2:$K$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0.998914092664093</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.654404981549815</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.985632183890805</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.000769230769231</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.983985260770975</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.95565749235474</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.998632135692139</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.983552631347368</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.076432702418507</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.996080954609265</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.986301370463014</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.979046242760116</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.995928338762215</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.997596153879808</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.002139364303178</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.9890625000125</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="0.00">
+                  <c:v>0.967359497205737</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="583300984"/>
+        <c:axId val="583342056"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="583300984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="low"/>
+        <c:txPr>
+          <a:bodyPr rot="-2700000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="583342056"/>
+        <c:crossesAt val="0.0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="9"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="583342056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.4"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="1"/>
+                  <a:t>Normalized</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" baseline="0"/>
+                  <a:t> Execution Time</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="583300984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
+        <c:minorUnit val="0.04"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.389475497124604"/>
+          <c:y val="0.923527144334896"/>
+          <c:w val="0.169442089205921"/>
+          <c:h val="0.0737075116168453"/>
         </c:manualLayout>
       </c:layout>
       <c:spPr>
@@ -1153,16 +1921,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>93134</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>63501</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>740834</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>93134</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1301,6 +2069,137 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
             <a:t>11.4</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>143945</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>59267</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>300579</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>59268</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.15223</cdr:x>
+      <cdr:y>0.15217</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.19029</cdr:x>
+      <cdr:y>0.24456</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1286933" y="474133"/>
+          <a:ext cx="321778" cy="287845"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="3175" cmpd="sng">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>2.3</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -1633,740 +2532,738 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="K17" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="8" max="8" width="7.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="B1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3">
         <v>10.32375</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>10.35</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>10.36</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="1"/>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" s="1">
-        <f t="shared" ref="H2:H18" si="0">C2/B2</f>
+      <c r="H2" s="7">
+        <f>C2/B2</f>
         <v>1.0025426807119506</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="6">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="5">
         <v>10.5425</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>11.69</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>86.72</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="7" t="s">
-        <v>0</v>
+      <c r="E3" s="1"/>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3" s="1">
-        <f t="shared" si="0"/>
+      <c r="H3" s="7">
+        <f>C3/B3</f>
         <v>1.1088451505809815</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="5">
         <v>1.36624999996</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>1.39</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>1.74</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="7" t="s">
-        <v>1</v>
+      <c r="E4" s="1"/>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4" s="1">
-        <f t="shared" si="0"/>
+      <c r="H4" s="7">
+        <f>C4/B4</f>
         <v>1.0173833486116708</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="6">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5">
         <v>6.2850000000000001</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>6.4980000000000002</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>6.5</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3" t="s">
-        <v>16</v>
+      <c r="E5" s="1"/>
+      <c r="F5" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
-      <c r="H5" s="1">
-        <f t="shared" si="0"/>
+      <c r="H5" s="7">
+        <f>C5/B5</f>
         <v>1.0338902147971361</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="6">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5">
         <v>1.5487500000700001</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>2.2799999999999998</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>17.64</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3" t="s">
-        <v>17</v>
+      <c r="E6" s="1"/>
+      <c r="F6" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="H6" s="1">
-        <f t="shared" si="0"/>
+      <c r="H6" s="7">
+        <f>C6/B6</f>
         <v>1.4721549636138491</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="6">
+        <v>19</v>
+      </c>
+      <c r="B7" s="5">
         <v>0.425000000047</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>0.32200000000000001</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>0.32700000000000001</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="1"/>
       <c r="F7" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
-      <c r="H7" s="1">
-        <f t="shared" si="0"/>
+      <c r="H7" s="7">
+        <f>C7/B7</f>
         <v>0.75764705873974258</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="6">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="5">
         <v>8.9350000000600005</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>11.475</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>11.56</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="7" t="s">
-        <v>6</v>
+      <c r="E8" s="1"/>
+      <c r="F8" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
-      <c r="H8" s="1">
-        <f t="shared" si="0"/>
+      <c r="H8" s="7">
+        <f>C8/B8</f>
         <v>1.2842753217597025</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="6">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5">
         <v>3.26124999998</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>0.37</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>0.38</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="1"/>
       <c r="F9" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="H9" s="1">
-        <f t="shared" si="0"/>
+      <c r="H9" s="7">
+        <f>C9/B9</f>
         <v>0.1134534304338119</v>
       </c>
       <c r="J9" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="5">
+        <v>19.061250000000001</v>
+      </c>
+      <c r="C10" s="5">
+        <v>19.03</v>
+      </c>
+      <c r="D10" s="1">
+        <v>19.02</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="7">
+        <f>C10/B10</f>
+        <v>0.99836054823267095</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="6">
-        <v>19.061250000000001</v>
-      </c>
-      <c r="C10" s="6">
-        <v>19.03</v>
-      </c>
-      <c r="D10" s="2">
-        <v>19.02</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" t="s">
+      <c r="B11" s="5">
+        <v>1.7989999999999999</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2.04</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10" s="1">
-        <f t="shared" si="0"/>
-        <v>0.99836054823267095</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="6">
-        <v>1.7989999999999999</v>
-      </c>
-      <c r="C11" s="6">
-        <v>1.8</v>
-      </c>
-      <c r="D11" s="5">
-        <v>2.04</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="5">
-        <v>1</v>
-      </c>
-      <c r="H11" s="1">
-        <f t="shared" si="0"/>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="H11" s="7">
+        <f>C11/B11</f>
         <v>1.0005558643690939</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="6">
+        <v>23</v>
+      </c>
+      <c r="B12" s="5">
         <v>20.574999999999999</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>21.11</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>21.37</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="1"/>
       <c r="F12" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G12">
         <v>1</v>
       </c>
-      <c r="H12" s="1">
-        <f t="shared" si="0"/>
+      <c r="H12" s="7">
+        <f>C12/B12</f>
         <v>1.0260024301336574</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="6">
+      <c r="A13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="5">
         <v>0.42299999999999999</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>0.35899999999999999</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>0.36499999999999999</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>20</v>
+      <c r="F13" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
-      <c r="H13" s="1">
-        <f t="shared" si="0"/>
+      <c r="H13" s="7">
+        <f>C13/B13</f>
         <v>0.84869976359338062</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="6">
+        <v>24</v>
+      </c>
+      <c r="B14" s="5">
         <v>2.0750000001900002</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>2.6</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>3.46</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="1"/>
       <c r="F14" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
-      <c r="H14" s="1">
-        <f t="shared" si="0"/>
+      <c r="H14" s="7">
+        <f>C14/B14</f>
         <v>1.2530120480780373</v>
       </c>
       <c r="J14" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="6">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="5">
         <v>2.7787500000600001</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>2.6</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>3.07</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="7" t="s">
-        <v>2</v>
+      <c r="E15" s="1"/>
+      <c r="F15" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
-      <c r="H15" s="1">
-        <f t="shared" si="0"/>
+      <c r="H15" s="7">
+        <f>C15/B15</f>
         <v>0.93567251459967959</v>
       </c>
       <c r="J15" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="6">
+        <v>25</v>
+      </c>
+      <c r="B16" s="5">
         <v>3.4037500002900001</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>2.04</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>2.08</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="1"/>
       <c r="F16" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
-      <c r="H16" s="1">
-        <f t="shared" si="0"/>
+      <c r="H16" s="7">
+        <f>C16/B16</f>
         <v>0.59933896432646105</v>
       </c>
       <c r="J16" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="6">
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="5">
         <v>4.2337500001299997</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>3.99</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>4.09</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="7" t="s">
-        <v>4</v>
+      <c r="E17" s="1"/>
+      <c r="F17" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
-      <c r="H17" s="8">
-        <f t="shared" si="0"/>
+      <c r="H17" s="7">
+        <f>C17/B17</f>
         <v>0.94242692645467607</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="6">
+        <v>26</v>
+      </c>
+      <c r="B18" s="5">
         <v>2.2000000001900002</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>2.3025000000000002</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>2.4</v>
       </c>
-      <c r="E18" s="2"/>
+      <c r="E18" s="1"/>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="G18">
         <v>1</v>
       </c>
-      <c r="H18" s="8">
-        <f t="shared" si="0"/>
+      <c r="H18" s="7">
+        <f>C18/B18</f>
         <v>1.0465909090005217</v>
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="3"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="2"/>
-      <c r="F19" s="3"/>
-      <c r="H19" s="8"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="1"/>
+      <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:8">
       <c r="F20" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="G20">
         <f>GEOMEAN(G3,G18)</f>
         <v>1</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="7">
         <f>GEOMEAN(H3:H18)</f>
         <v>0.87321433294717998</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="B22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="8"/>
+        <v>6</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
-      <c r="C23" s="8">
-        <f t="shared" ref="C23:C31" si="1">D2/B2</f>
+      <c r="C23" s="7">
+        <f t="shared" ref="C23:C31" si="0">D2/B2</f>
         <v>1.0035113209831699</v>
       </c>
-      <c r="D23" s="8"/>
+      <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="7" t="s">
-        <v>0</v>
+      <c r="A24" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
-      <c r="C24" s="8">
-        <f t="shared" si="1"/>
+      <c r="C24" s="7">
+        <f t="shared" si="0"/>
         <v>8.2257529049087026</v>
       </c>
-      <c r="D24" s="8"/>
+      <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="7" t="s">
-        <v>1</v>
+      <c r="A25" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25" s="8">
-        <f t="shared" si="1"/>
+      <c r="C25" s="7">
+        <f t="shared" si="0"/>
         <v>1.2735590119311564</v>
       </c>
-      <c r="D25" s="8"/>
+      <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="3" t="s">
-        <v>16</v>
+      <c r="A26" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
-      <c r="C26" s="8">
-        <f t="shared" si="1"/>
+      <c r="C26" s="7">
+        <f t="shared" si="0"/>
         <v>1.0342084327764518</v>
       </c>
-      <c r="D26" s="8"/>
+      <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="3" t="s">
-        <v>17</v>
+      <c r="A27" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
-      <c r="C27" s="8">
-        <f t="shared" si="1"/>
+      <c r="C27" s="7">
+        <f t="shared" si="0"/>
         <v>11.389830507959781</v>
       </c>
-      <c r="D27" s="8"/>
+      <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
-      <c r="C28" s="8">
-        <f t="shared" si="1"/>
+      <c r="C28" s="7">
+        <f t="shared" si="0"/>
         <v>0.76941176462079452</v>
       </c>
-      <c r="D28" s="8"/>
+      <c r="D28" s="7"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="7" t="s">
-        <v>6</v>
+      <c r="A29" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
-      <c r="C29" s="8">
-        <f t="shared" si="1"/>
+      <c r="C29" s="7">
+        <f t="shared" si="0"/>
         <v>1.293788472291256</v>
       </c>
-      <c r="D29" s="8"/>
+      <c r="D29" s="7"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
-      <c r="C30" s="8">
-        <f t="shared" si="1"/>
+      <c r="C30" s="7">
+        <f t="shared" si="0"/>
         <v>0.11651973936445548</v>
       </c>
-      <c r="D30" s="8"/>
+      <c r="D30" s="7"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
-      <c r="C31" s="8">
-        <f t="shared" si="1"/>
+      <c r="C31" s="7">
+        <f t="shared" si="0"/>
         <v>0.99783592366712559</v>
       </c>
-      <c r="D31" s="8"/>
+      <c r="D31" s="7"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="3" t="s">
-        <v>19</v>
+      <c r="A32" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
-      <c r="C32" s="8">
+      <c r="C32" s="7">
         <f>D11/C11</f>
         <v>1.1333333333333333</v>
       </c>
-      <c r="D32" s="8"/>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
-      <c r="C33" s="8">
+      <c r="C33" s="7">
         <f>D12/B12</f>
         <v>1.0386391251518834</v>
       </c>
-      <c r="D33" s="8"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="3" t="s">
-        <v>20</v>
+      <c r="D33" s="7"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
-      <c r="C34" s="8">
+      <c r="C34" s="7">
         <f>D13/C13</f>
         <v>1.0167130919220055</v>
       </c>
-      <c r="D34" s="8"/>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="D34" s="7"/>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C35" s="7">
         <f>D14/B14</f>
         <v>1.6674698793653882</v>
       </c>
-      <c r="D35" s="8"/>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="7" t="s">
-        <v>2</v>
+      <c r="D35" s="7"/>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C36" s="7">
         <f>D15/B15</f>
         <v>1.1048133153157755</v>
       </c>
-      <c r="D36" s="8"/>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="D36" s="7"/>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37" s="7">
         <f>D16/B16</f>
         <v>0.61109070872501914</v>
       </c>
-      <c r="D37" s="8"/>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="7" t="s">
-        <v>4</v>
+      <c r="D37" s="7"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38" s="7">
         <f>D17/B17</f>
         <v>0.96604664892221181</v>
       </c>
-      <c r="D38" s="8"/>
-      <c r="H38" s="8"/>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="D38" s="7"/>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C39" s="7">
         <f>D18/B18</f>
         <v>1.090909090814876</v>
       </c>
-      <c r="D39" s="8"/>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="D39" s="7"/>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="B41">
         <f>GEOMEAN(B24,B39)</f>
         <v>1</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C41" s="7">
         <f>GEOMEAN(C24:C39)</f>
         <v>1.2069556167564377</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A23:C39">
-    <sortCondition ref="A24:A39"/>
+  <sortState ref="F2:H18">
+    <sortCondition descending="1" ref="H3:H18"/>
   </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2377,4 +3274,1022 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:K39"/>
+  <sheetViews>
+    <sheetView showRuler="0" topLeftCell="M1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1">
+        <v>10.36</v>
+      </c>
+      <c r="C2">
+        <v>10.376250000000001</v>
+      </c>
+      <c r="D2" s="1">
+        <v>10.36</v>
+      </c>
+      <c r="E2">
+        <v>10.348750000000001</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2">
+        <f>C2/B2</f>
+        <v>1.0015685328185329</v>
+      </c>
+      <c r="J2" s="7">
+        <f>B2/D2</f>
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <f>E2/B2</f>
+        <v>0.99891409266409281</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1">
+        <v>86.72</v>
+      </c>
+      <c r="C3">
+        <v>196.26</v>
+      </c>
+      <c r="D3" s="1">
+        <v>86.72</v>
+      </c>
+      <c r="E3">
+        <v>56.75</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I17" si="0">C3/B3</f>
+        <v>2.2631457564575643</v>
+      </c>
+      <c r="J3" s="7">
+        <f t="shared" ref="J3:J17" si="1">B3/D3</f>
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K17" si="2">E3/B3</f>
+        <v>0.65440498154981552</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.74</v>
+      </c>
+      <c r="C4">
+        <v>1.7450000001099999</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1.74</v>
+      </c>
+      <c r="E4">
+        <v>1.7149999999700001</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>1.002873563281609</v>
+      </c>
+      <c r="J4" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="2"/>
+        <v>0.98563218389080465</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="C5">
+        <v>6.5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="E5">
+        <v>6.5049999999999999</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J5" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="2"/>
+        <v>1.0007692307692309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="1">
+        <v>17.64</v>
+      </c>
+      <c r="C6">
+        <v>17.107500000000002</v>
+      </c>
+      <c r="D6" s="1">
+        <v>17.64</v>
+      </c>
+      <c r="E6">
+        <v>17.357500000000002</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>0.96981292517006812</v>
+      </c>
+      <c r="J6" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>0.98398526077097515</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="C7">
+        <v>0.3125</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="E7">
+        <v>0.3125</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>0.95565749235474007</v>
+      </c>
+      <c r="J7" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>0.95565749235474007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1">
+        <v>13.7075</v>
+      </c>
+      <c r="C8">
+        <v>13.7325</v>
+      </c>
+      <c r="D8" s="1">
+        <v>13.7075</v>
+      </c>
+      <c r="E8">
+        <v>13.688750000000001</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>1.0018238190771476</v>
+      </c>
+      <c r="J8" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>0.99863213569213938</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="C9">
+        <v>0.38125000009299997</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="E9">
+        <v>0.37374999991199997</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>1.0032894739289473</v>
+      </c>
+      <c r="J9" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>0.98355263134736837</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1">
+        <v>19.02</v>
+      </c>
+      <c r="C10">
+        <v>20.11375</v>
+      </c>
+      <c r="D10" s="1">
+        <v>19.02</v>
+      </c>
+      <c r="E10">
+        <v>20.473749999999999</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>1.0575052576235542</v>
+      </c>
+      <c r="J10" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>1.0764327024185067</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1">
+        <v>21.37</v>
+      </c>
+      <c r="C11">
+        <v>21.717499999899999</v>
+      </c>
+      <c r="D11" s="1">
+        <v>21.37</v>
+      </c>
+      <c r="E11">
+        <v>21.286249999999999</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>1.0162611137061299</v>
+      </c>
+      <c r="J11" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>0.99608095460926527</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="C12">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="E12">
+        <v>0.36000000021900003</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>0.98356164383561639</v>
+      </c>
+      <c r="J12" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="2"/>
+        <v>0.9863013704630138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3.46</v>
+      </c>
+      <c r="C13">
+        <v>3.3925000000700001</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3.46</v>
+      </c>
+      <c r="E13">
+        <v>3.3874999999500002</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>0.98049132950000006</v>
+      </c>
+      <c r="J13" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>0.97904624276011565</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3.07</v>
+      </c>
+      <c r="C14">
+        <v>2.9975000000600001</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3.07</v>
+      </c>
+      <c r="E14">
+        <v>3.0575000000000001</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>0.97638436484039093</v>
+      </c>
+      <c r="J14" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="2"/>
+        <v>0.99592833876221509</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2.08</v>
+      </c>
+      <c r="C15">
+        <v>2.08250000002</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2.08</v>
+      </c>
+      <c r="E15">
+        <v>2.0750000000700002</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>1.0012019230865383</v>
+      </c>
+      <c r="J15" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="2"/>
+        <v>0.99759615387980771</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1">
+        <v>4.09</v>
+      </c>
+      <c r="C16">
+        <v>4.1099999999900003</v>
+      </c>
+      <c r="D16" s="1">
+        <v>4.09</v>
+      </c>
+      <c r="E16">
+        <v>4.0987499999999999</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>1.0048899755476774</v>
+      </c>
+      <c r="J16" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="2"/>
+        <v>1.0021393643031784</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="C17">
+        <v>2.4112499999999999</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="E17">
+        <v>2.3737500000299998</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>1.0046875</v>
+      </c>
+      <c r="J17" s="7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="2"/>
+        <v>0.98906250001249996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="2"/>
+      <c r="B18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="H19" t="s">
+        <v>30</v>
+      </c>
+      <c r="I19">
+        <f>GEOMEAN(I2,I17)</f>
+        <v>1.003126804205789</v>
+      </c>
+      <c r="J19" s="7">
+        <f>GEOMEAN(J3:J17)</f>
+        <v>1</v>
+      </c>
+      <c r="K19" s="7">
+        <f>GEOMEAN(K3:K17)</f>
+        <v>0.96735949720573722</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="8">
+        <v>0</v>
+      </c>
+      <c r="C22" s="8">
+        <v>0</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0</v>
+      </c>
+      <c r="E22" s="8">
+        <v>0</v>
+      </c>
+      <c r="F22" s="8">
+        <v>0</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="8">
+        <v>1</v>
+      </c>
+      <c r="C23" s="8">
+        <v>21444321</v>
+      </c>
+      <c r="D23" s="9">
+        <v>1</v>
+      </c>
+      <c r="E23" s="8">
+        <v>26369324</v>
+      </c>
+      <c r="F23" s="8">
+        <v>1</v>
+      </c>
+      <c r="G23" s="8">
+        <v>30580451</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="8">
+        <v>0</v>
+      </c>
+      <c r="C24" s="8">
+        <v>0</v>
+      </c>
+      <c r="D24" s="9">
+        <v>0</v>
+      </c>
+      <c r="E24" s="8">
+        <v>0</v>
+      </c>
+      <c r="F24" s="8">
+        <v>0</v>
+      </c>
+      <c r="G24" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="8">
+        <v>1</v>
+      </c>
+      <c r="C25" s="8">
+        <v>3</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+      <c r="E25" s="8">
+        <v>0</v>
+      </c>
+      <c r="F25" s="8">
+        <v>0</v>
+      </c>
+      <c r="G25" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="8">
+        <v>1</v>
+      </c>
+      <c r="C26" s="8">
+        <v>3370</v>
+      </c>
+      <c r="D26" s="9">
+        <v>1</v>
+      </c>
+      <c r="E26" s="8">
+        <v>4064</v>
+      </c>
+      <c r="F26" s="8">
+        <v>1</v>
+      </c>
+      <c r="G26" s="8">
+        <v>2851</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="8">
+        <v>0</v>
+      </c>
+      <c r="C27" s="8">
+        <v>0</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0</v>
+      </c>
+      <c r="E27" s="8">
+        <v>0</v>
+      </c>
+      <c r="F27" s="8">
+        <v>0</v>
+      </c>
+      <c r="G27" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="8">
+        <v>2</v>
+      </c>
+      <c r="C28" s="8">
+        <v>2974</v>
+      </c>
+      <c r="D28" s="9">
+        <v>2</v>
+      </c>
+      <c r="E28" s="8">
+        <v>1122</v>
+      </c>
+      <c r="F28" s="8">
+        <v>1</v>
+      </c>
+      <c r="G28" s="8">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="8">
+        <v>1</v>
+      </c>
+      <c r="C29" s="8">
+        <v>1050</v>
+      </c>
+      <c r="D29" s="9">
+        <v>1</v>
+      </c>
+      <c r="E29" s="8">
+        <v>311</v>
+      </c>
+      <c r="F29" s="8">
+        <v>1</v>
+      </c>
+      <c r="G29" s="8">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="8">
+        <v>0</v>
+      </c>
+      <c r="C30" s="8">
+        <v>0</v>
+      </c>
+      <c r="D30" s="9">
+        <v>0</v>
+      </c>
+      <c r="E30" s="8">
+        <v>0</v>
+      </c>
+      <c r="F30" s="8">
+        <v>0</v>
+      </c>
+      <c r="G30" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="A31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="8">
+        <v>0</v>
+      </c>
+      <c r="C31" s="8">
+        <v>0</v>
+      </c>
+      <c r="D31" s="9">
+        <v>0</v>
+      </c>
+      <c r="E31" s="8">
+        <v>0</v>
+      </c>
+      <c r="F31" s="8">
+        <v>0</v>
+      </c>
+      <c r="G31" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="A32" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="8">
+        <v>0</v>
+      </c>
+      <c r="C32" s="8">
+        <v>0</v>
+      </c>
+      <c r="D32" s="9">
+        <v>0</v>
+      </c>
+      <c r="E32" s="8">
+        <v>0</v>
+      </c>
+      <c r="F32" s="8">
+        <v>0</v>
+      </c>
+      <c r="G32" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="8">
+        <v>5</v>
+      </c>
+      <c r="C33" s="8">
+        <v>14494</v>
+      </c>
+      <c r="D33" s="9">
+        <v>5</v>
+      </c>
+      <c r="E33" s="8">
+        <v>14782</v>
+      </c>
+      <c r="F33" s="8">
+        <v>5</v>
+      </c>
+      <c r="G33" s="8">
+        <v>14891</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="8">
+        <v>2</v>
+      </c>
+      <c r="C34" s="8">
+        <v>52462</v>
+      </c>
+      <c r="D34" s="9">
+        <v>1</v>
+      </c>
+      <c r="E34" s="8">
+        <v>52283</v>
+      </c>
+      <c r="F34" s="8">
+        <v>1</v>
+      </c>
+      <c r="G34" s="8">
+        <v>52450</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="8">
+        <v>0</v>
+      </c>
+      <c r="C35" s="8">
+        <v>0</v>
+      </c>
+      <c r="D35" s="9">
+        <v>0</v>
+      </c>
+      <c r="E35" s="8">
+        <v>0</v>
+      </c>
+      <c r="F35" s="8">
+        <v>0</v>
+      </c>
+      <c r="G35" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="8">
+        <v>0</v>
+      </c>
+      <c r="C36" s="8">
+        <v>0</v>
+      </c>
+      <c r="D36" s="9">
+        <v>0</v>
+      </c>
+      <c r="E36" s="8">
+        <v>0</v>
+      </c>
+      <c r="F36" s="8">
+        <v>0</v>
+      </c>
+      <c r="G36" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B37" s="8">
+        <v>4</v>
+      </c>
+      <c r="C37" s="8">
+        <v>9849</v>
+      </c>
+      <c r="D37" s="9">
+        <v>4</v>
+      </c>
+      <c r="E37" s="8">
+        <v>2699</v>
+      </c>
+      <c r="F37" s="8">
+        <v>3</v>
+      </c>
+      <c r="G37" s="8">
+        <v>622</v>
+      </c>
+      <c r="I37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="B38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>